<commit_message>
Integrate Alpaca trade execution logic and update SPY data fetch
</commit_message>
<xml_diff>
--- a/spy_daily_data.xlsx
+++ b/spy_daily_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S59"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3300,6 +3300,61 @@
       </c>
       <c r="S59" t="inlineStr"/>
     </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45744.16666666666</v>
+      </c>
+      <c r="B60" t="n">
+        <v>565.53</v>
+      </c>
+      <c r="C60" t="n">
+        <v>566.2675</v>
+      </c>
+      <c r="D60" t="n">
+        <v>555.0700000000001</v>
+      </c>
+      <c r="E60" t="n">
+        <v>555.66</v>
+      </c>
+      <c r="F60" t="n">
+        <v>71628953</v>
+      </c>
+      <c r="G60" t="n">
+        <v>516430404000</v>
+      </c>
+      <c r="H60" t="n">
+        <v>566.564</v>
+      </c>
+      <c r="I60" t="n">
+        <v>567.3779999999999</v>
+      </c>
+      <c r="J60" t="n">
+        <v>578.5740000000001</v>
+      </c>
+      <c r="K60" t="n">
+        <v>588.4064000000001</v>
+      </c>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="n">
+        <v>-6.537610499655671</v>
+      </c>
+      <c r="N60" t="n">
+        <v>-7.313184492112273</v>
+      </c>
+      <c r="O60" t="n">
+        <v>42.99157028033723</v>
+      </c>
+      <c r="P60" t="n">
+        <v>35.17092700954727</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>34.1669106881405</v>
+      </c>
+      <c r="R60" t="n">
+        <v>42.44607244607244</v>
+      </c>
+      <c r="S60" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>